<commit_message>
Repeated experiments with CPU_MHZ correctly set
</commit_message>
<xml_diff>
--- a/doc/riscv-benchmarks-results.xlsx
+++ b/doc/riscv-benchmarks-results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianluca/VirtualBox VMs/Shared/aftab-cfi-pla/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gianluca/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2FAE7A-EC17-B040-AC81-4F545E61A37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1076DA58-4CE4-724C-AB52-2A2608740F76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="1120" windowWidth="31220" windowHeight="17440" xr2:uid="{6C163CD9-0266-BA4D-8209-435E9226B323}"/>
   </bookViews>
@@ -244,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -256,6 +256,7 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -570,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBDF4BAC-6269-AF4A-97B2-FFF761B3352E}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -581,10 +582,12 @@
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
     <col min="6" max="7" width="13.5" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" customWidth="1"/>
     <col min="12" max="12" width="13.1640625" customWidth="1"/>
     <col min="13" max="13" width="14.6640625" customWidth="1"/>
@@ -651,15 +654,15 @@
         <v>1151</v>
       </c>
       <c r="C2" s="6">
-        <v>37559971</v>
+        <v>3755997163</v>
       </c>
       <c r="D2" s="6">
         <f>C2-B2</f>
-        <v>37558820</v>
+        <v>3755996012</v>
       </c>
       <c r="E2" s="6">
         <f>(D2*10)/1000000000</f>
-        <v>0.37558819999999998</v>
+        <v>37.55996012</v>
       </c>
       <c r="F2" s="6">
         <v>3056</v>
@@ -671,15 +674,15 @@
         <v>1151</v>
       </c>
       <c r="I2" s="7">
-        <v>37559971</v>
+        <v>3755997163</v>
       </c>
       <c r="J2" s="7">
         <f>I2-H2</f>
-        <v>37558820</v>
+        <v>3755996012</v>
       </c>
       <c r="K2" s="7">
         <f>(J2*10)/1000000000</f>
-        <v>0.37558819999999998</v>
+        <v>37.55996012</v>
       </c>
       <c r="L2" s="7">
         <v>3056</v>
@@ -708,15 +711,15 @@
         <v>1347</v>
       </c>
       <c r="C3" s="6">
-        <v>41097572</v>
+        <v>4109757230</v>
       </c>
       <c r="D3" s="6">
         <f t="shared" ref="D3:D23" si="0">C3-B3</f>
-        <v>41096225</v>
+        <v>4109755883</v>
       </c>
       <c r="E3" s="6">
         <f t="shared" ref="E3:E23" si="1">(D3*10)/1000000000</f>
-        <v>0.41096224999999997</v>
+        <v>41.097558829999997</v>
       </c>
       <c r="F3" s="6">
         <v>22968</v>
@@ -728,15 +731,15 @@
         <v>1347</v>
       </c>
       <c r="I3" s="7">
-        <v>41097620</v>
+        <v>4110237245.7363024</v>
       </c>
       <c r="J3" s="7">
         <f t="shared" ref="J3:J23" si="2">I3-H3</f>
-        <v>41096273</v>
+        <v>4110235898.7363024</v>
       </c>
       <c r="K3" s="7">
         <f t="shared" ref="K3:K23" si="3">(J3*10)/1000000000</f>
-        <v>0.41096273</v>
+        <v>41.102358987363019</v>
       </c>
       <c r="L3" s="7">
         <v>23280</v>
@@ -746,7 +749,7 @@
       </c>
       <c r="N3" s="8">
         <f t="shared" ref="N3:N23" si="4">(K3*100/E3)-100</f>
-        <v>1.1679904905292915E-4</v>
+        <v>1.1679908733469802E-2</v>
       </c>
       <c r="O3" s="8">
         <f t="shared" ref="O3:O23" si="5">(L3*100/F3)-100</f>
@@ -765,15 +768,15 @@
         <v>1437</v>
       </c>
       <c r="C4" s="6">
-        <v>75481460</v>
+        <v>7548146043</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="0"/>
-        <v>75480023</v>
+        <v>7548144606</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" si="1"/>
-        <v>0.75480022999999996</v>
+        <v>75.481446059999996</v>
       </c>
       <c r="F4" s="6">
         <v>49624</v>
@@ -785,15 +788,15 @@
         <v>1437</v>
       </c>
       <c r="I4" s="7">
-        <v>75533684</v>
+        <v>8070395988.4585695</v>
       </c>
       <c r="J4" s="7">
         <f t="shared" si="2"/>
-        <v>75532247</v>
+        <v>8070394551.4585695</v>
       </c>
       <c r="K4" s="7">
         <f t="shared" si="3"/>
-        <v>0.75532246999999997</v>
+        <v>80.703945514585698</v>
       </c>
       <c r="L4" s="7">
         <v>50388</v>
@@ -803,7 +806,7 @@
       </c>
       <c r="N4" s="8">
         <f t="shared" si="4"/>
-        <v>6.9189168106106536E-2</v>
+        <v>6.9189181278195804</v>
       </c>
       <c r="O4" s="8">
         <f t="shared" si="5"/>
@@ -822,15 +825,15 @@
         <v>12805</v>
       </c>
       <c r="C5" s="6">
-        <v>51679071</v>
+        <v>5167907133</v>
       </c>
       <c r="D5" s="6">
         <f t="shared" si="0"/>
-        <v>51666266</v>
+        <v>5167894328</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="1"/>
-        <v>0.51666266000000005</v>
+        <v>51.678943279999999</v>
       </c>
       <c r="F5" s="6">
         <v>4016</v>
@@ -842,15 +845,15 @@
         <v>12805</v>
       </c>
       <c r="I5" s="7">
-        <v>51679071</v>
+        <v>5167907133</v>
       </c>
       <c r="J5" s="7">
         <f t="shared" si="2"/>
-        <v>51666266</v>
+        <v>5167894328</v>
       </c>
       <c r="K5" s="7">
         <f t="shared" si="3"/>
-        <v>0.51666266000000005</v>
+        <v>51.678943279999999</v>
       </c>
       <c r="L5" s="7">
         <v>4016</v>
@@ -879,15 +882,15 @@
         <v>64451</v>
       </c>
       <c r="C6" s="6">
-        <v>20878286</v>
+        <v>2087828612</v>
       </c>
       <c r="D6" s="6">
         <f t="shared" si="0"/>
-        <v>20813835</v>
+        <v>2087764161</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="1"/>
-        <v>0.20813835</v>
+        <v>20.877641610000001</v>
       </c>
       <c r="F6" s="6">
         <v>27768</v>
@@ -899,15 +902,15 @@
         <v>64451</v>
       </c>
       <c r="I6" s="7">
-        <v>20878510</v>
+        <v>2090075548.276222</v>
       </c>
       <c r="J6" s="7">
         <f t="shared" si="2"/>
-        <v>20814059</v>
+        <v>2090011097.276222</v>
       </c>
       <c r="K6" s="7">
         <f t="shared" si="3"/>
-        <v>0.20814058999999999</v>
+        <v>20.900110972762217</v>
       </c>
       <c r="L6" s="7">
         <v>28080</v>
@@ -917,7 +920,7 @@
       </c>
       <c r="N6" s="8">
         <f t="shared" si="4"/>
-        <v>1.0762072438836867E-3</v>
+        <v>0.10762404672878745</v>
       </c>
       <c r="O6" s="8">
         <f t="shared" si="5"/>
@@ -936,15 +939,15 @@
         <v>175097</v>
       </c>
       <c r="C7" s="6">
-        <v>54463016</v>
+        <v>5446301669</v>
       </c>
       <c r="D7" s="6">
         <f t="shared" si="0"/>
-        <v>54287919</v>
+        <v>5446126572</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="1"/>
-        <v>0.54287918999999996</v>
+        <v>54.46126572</v>
       </c>
       <c r="F7" s="6">
         <v>1904</v>
@@ -956,15 +959,15 @@
         <v>175097</v>
       </c>
       <c r="I7" s="7">
-        <v>54463016</v>
+        <v>5446301669</v>
       </c>
       <c r="J7" s="7">
         <f t="shared" si="2"/>
-        <v>54287919</v>
+        <v>5446126572</v>
       </c>
       <c r="K7" s="7">
         <f t="shared" si="3"/>
-        <v>0.54287918999999996</v>
+        <v>54.46126572</v>
       </c>
       <c r="L7" s="7">
         <v>1976</v>
@@ -993,15 +996,15 @@
         <v>23793</v>
       </c>
       <c r="C8" s="6">
-        <v>17058399</v>
+        <v>1705839944</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
-        <v>17034606</v>
+        <v>1705816151</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" si="1"/>
-        <v>0.17034605999999999</v>
+        <v>17.058161510000001</v>
       </c>
       <c r="F8" s="6">
         <v>23752</v>
@@ -1013,15 +1016,15 @@
         <v>23793</v>
       </c>
       <c r="I8" s="7">
-        <v>17059311</v>
+        <v>1714972682.549557</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="2"/>
-        <v>17035518</v>
+        <v>1714948889.549557</v>
       </c>
       <c r="K8" s="7">
         <f t="shared" si="3"/>
-        <v>0.17035517999999999</v>
+        <v>17.149488895495569</v>
       </c>
       <c r="L8" s="7">
         <v>24064</v>
@@ -1031,7 +1034,7 @@
       </c>
       <c r="N8" s="8">
         <f t="shared" si="4"/>
-        <v>5.3538074200218944E-3</v>
+        <v>0.5353882095794944</v>
       </c>
       <c r="O8" s="8">
         <f t="shared" si="5"/>
@@ -1050,15 +1053,15 @@
         <v>19595</v>
       </c>
       <c r="C9" s="6">
-        <v>26231500</v>
+        <v>2623150048</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="0"/>
-        <v>26211905</v>
+        <v>2623130453</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="1"/>
-        <v>0.26211905000000002</v>
+        <v>26.231304529999999</v>
       </c>
       <c r="F9" s="6">
         <v>15680</v>
@@ -1070,15 +1073,15 @@
         <v>19595</v>
       </c>
       <c r="I9" s="7">
-        <v>26240380</v>
+        <v>2712016433.0499949</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="2"/>
-        <v>26220785</v>
+        <v>2711996838.0499949</v>
       </c>
       <c r="K9" s="7">
         <f t="shared" si="3"/>
-        <v>0.26220785000000002</v>
+        <v>27.119968380499952</v>
       </c>
       <c r="L9" s="7">
         <v>15688</v>
@@ -1088,7 +1091,7 @@
       </c>
       <c r="N9" s="8">
         <f t="shared" si="4"/>
-        <v>3.3877736089763744E-2</v>
+        <v>3.3877989159235682</v>
       </c>
       <c r="O9" s="8">
         <f t="shared" si="5"/>
@@ -1107,15 +1110,15 @@
         <v>1118</v>
       </c>
       <c r="C10" s="6">
-        <v>31894191</v>
+        <v>3189419155</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="0"/>
-        <v>31893073</v>
+        <v>3189418037</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="1"/>
-        <v>0.31893073</v>
+        <v>31.894180370000001</v>
       </c>
       <c r="F10" s="6">
         <v>15244</v>
@@ -1127,15 +1130,15 @@
         <v>1118</v>
       </c>
       <c r="I10" s="7">
-        <v>31894231</v>
+        <v>3189819169.0287313</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="2"/>
-        <v>31893113</v>
+        <v>3189818051.0287313</v>
       </c>
       <c r="K10" s="7">
         <f t="shared" si="3"/>
-        <v>0.31893113000000001</v>
+        <v>31.898180510287315</v>
       </c>
       <c r="L10" s="7">
         <v>15260</v>
@@ -1145,7 +1148,7 @@
       </c>
       <c r="N10" s="8">
         <f t="shared" si="4"/>
-        <v>1.2541908394325674E-4</v>
+        <v>1.2541912790709375E-2</v>
       </c>
       <c r="O10" s="8">
         <f t="shared" si="5"/>
@@ -1164,15 +1167,15 @@
         <v>8017</v>
       </c>
       <c r="C11" s="6">
-        <v>40327634</v>
+        <v>4032763475</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="0"/>
-        <v>40319617</v>
+        <v>4032755458</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="1"/>
-        <v>0.40319617000000002</v>
+        <v>40.327554579999997</v>
       </c>
       <c r="F11" s="6">
         <v>7468</v>
@@ -1184,15 +1187,15 @@
         <v>8017</v>
       </c>
       <c r="I11" s="7">
-        <v>40327634</v>
+        <v>4032763475</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="2"/>
-        <v>40319617</v>
+        <v>4032755458</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="3"/>
-        <v>0.40319617000000002</v>
+        <v>40.327554579999997</v>
       </c>
       <c r="L11" s="7">
         <v>7508</v>
@@ -1221,15 +1224,15 @@
         <v>1379</v>
       </c>
       <c r="C12" s="6">
-        <v>34526050</v>
+        <v>3452605083</v>
       </c>
       <c r="D12" s="6">
         <f t="shared" si="0"/>
-        <v>34524671</v>
+        <v>3452603704</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="1"/>
-        <v>0.34524671000000001</v>
+        <v>34.526037039999999</v>
       </c>
       <c r="F12" s="6">
         <v>11544</v>
@@ -1241,15 +1244,15 @@
         <v>1379</v>
       </c>
       <c r="I12" s="7">
-        <v>34541250</v>
+        <v>3604611157.9068036</v>
       </c>
       <c r="J12" s="7">
         <f t="shared" si="2"/>
-        <v>34539871</v>
+        <v>3604609778.9068036</v>
       </c>
       <c r="K12" s="7">
         <f t="shared" si="3"/>
-        <v>0.34539871</v>
+        <v>36.046097789068035</v>
       </c>
       <c r="L12" s="7">
         <v>11656</v>
@@ -1259,7 +1262,7 @@
       </c>
       <c r="N12" s="8">
         <f t="shared" si="4"/>
-        <v>4.4026487609386322E-2</v>
+        <v>4.4026505193948964</v>
       </c>
       <c r="O12" s="8">
         <f t="shared" si="5"/>
@@ -1278,15 +1281,15 @@
         <v>1210</v>
       </c>
       <c r="C13" s="6">
-        <v>25270107</v>
+        <v>2527010749</v>
       </c>
       <c r="D13" s="6">
         <f t="shared" si="0"/>
-        <v>25268897</v>
+        <v>2527009539</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="1"/>
-        <v>0.25268897000000001</v>
+        <v>25.270095390000002</v>
       </c>
       <c r="F13" s="6">
         <v>19632</v>
@@ -1298,15 +1301,15 @@
         <v>1210</v>
       </c>
       <c r="I13" s="7">
-        <v>25270107</v>
+        <v>2527010749</v>
       </c>
       <c r="J13" s="7">
         <f t="shared" si="2"/>
-        <v>25268897</v>
+        <v>2527009539</v>
       </c>
       <c r="K13" s="7">
         <f t="shared" si="3"/>
-        <v>0.25268897000000001</v>
+        <v>25.270095390000002</v>
       </c>
       <c r="L13" s="7">
         <v>19632</v>
@@ -1335,15 +1338,15 @@
         <v>18254</v>
       </c>
       <c r="C14" s="6">
-        <v>36351114</v>
+        <v>3635111428</v>
       </c>
       <c r="D14" s="6">
         <f t="shared" si="0"/>
-        <v>36332860</v>
+        <v>3635093174</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" si="1"/>
-        <v>0.3633286</v>
+        <v>36.35093174</v>
       </c>
       <c r="F14" s="6">
         <v>24148</v>
@@ -1355,15 +1358,15 @@
         <v>18254</v>
       </c>
       <c r="I14" s="7">
-        <v>36367530</v>
+        <v>3799353904.9259934</v>
       </c>
       <c r="J14" s="7">
         <f t="shared" si="2"/>
-        <v>36349276</v>
+        <v>3799335650.9259934</v>
       </c>
       <c r="K14" s="7">
         <f t="shared" si="3"/>
-        <v>0.36349276000000003</v>
+        <v>37.993356509259932</v>
       </c>
       <c r="L14" s="7">
         <v>24212</v>
@@ -1373,7 +1376,7 @@
       </c>
       <c r="N14" s="8">
         <f t="shared" si="4"/>
-        <v>4.5182239988818651E-2</v>
+        <v>4.5182466876155303</v>
       </c>
       <c r="O14" s="8">
         <f t="shared" si="5"/>
@@ -1392,15 +1395,15 @@
         <v>738</v>
       </c>
       <c r="C15" s="6">
-        <v>22015043</v>
+        <v>2201504365</v>
       </c>
       <c r="D15" s="6">
         <f t="shared" si="0"/>
-        <v>22014305</v>
+        <v>2201503627</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" si="1"/>
-        <v>0.22014305000000001</v>
+        <v>22.01503627</v>
       </c>
       <c r="F15" s="6">
         <v>360</v>
@@ -1412,15 +1415,15 @@
         <v>738</v>
       </c>
       <c r="I15" s="7">
-        <v>22015043</v>
+        <v>2201504365</v>
       </c>
       <c r="J15" s="7">
         <f t="shared" si="2"/>
-        <v>22014305</v>
+        <v>2201503627</v>
       </c>
       <c r="K15" s="7">
         <f t="shared" si="3"/>
-        <v>0.22014305000000001</v>
+        <v>22.01503627</v>
       </c>
       <c r="L15" s="7">
         <v>360</v>
@@ -1449,15 +1452,15 @@
         <v>61029</v>
       </c>
       <c r="C16" s="6">
-        <v>27738809</v>
+        <v>2773880934</v>
       </c>
       <c r="D16" s="6">
         <f t="shared" si="0"/>
-        <v>27677780</v>
+        <v>2773819905</v>
       </c>
       <c r="E16" s="6">
         <f t="shared" si="1"/>
-        <v>0.27677780000000002</v>
+        <v>27.738199049999999</v>
       </c>
       <c r="F16" s="6">
         <v>42460</v>
@@ -1469,15 +1472,15 @@
         <v>61029</v>
       </c>
       <c r="I16" s="7">
-        <v>27739913</v>
+        <v>2784945277.1341786</v>
       </c>
       <c r="J16" s="7">
         <f t="shared" si="2"/>
-        <v>27678884</v>
+        <v>2784884248.1341786</v>
       </c>
       <c r="K16" s="7">
         <f t="shared" si="3"/>
-        <v>0.27678883999999998</v>
+        <v>27.848842481341787</v>
       </c>
       <c r="L16" s="7">
         <v>42724</v>
@@ -1487,7 +1490,7 @@
       </c>
       <c r="N16" s="8">
         <f t="shared" si="4"/>
-        <v>3.9887592140530614E-3</v>
+        <v>0.39888469738912136</v>
       </c>
       <c r="O16" s="8">
         <f t="shared" si="5"/>
@@ -1506,15 +1509,15 @@
         <v>64642</v>
       </c>
       <c r="C17" s="6">
-        <v>23826293</v>
+        <v>2382629385</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="0"/>
-        <v>23761651</v>
+        <v>2382564743</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="1"/>
-        <v>0.23761651</v>
+        <v>23.82564743</v>
       </c>
       <c r="F17" s="6">
         <v>37572</v>
@@ -1526,15 +1529,15 @@
         <v>64642</v>
       </c>
       <c r="I17" s="7">
-        <v>23826341</v>
+        <v>2383110690.8254185</v>
       </c>
       <c r="J17" s="7">
         <f t="shared" si="2"/>
-        <v>23761699</v>
+        <v>2383046048.8254185</v>
       </c>
       <c r="K17" s="7">
         <f t="shared" si="3"/>
-        <v>0.23761699</v>
+        <v>23.830460488254186</v>
       </c>
       <c r="L17" s="7">
         <v>37972</v>
@@ -1544,7 +1547,7 @@
       </c>
       <c r="N17" s="8">
         <f t="shared" si="4"/>
-        <v>2.0200616530985371E-4</v>
+        <v>2.0201164599299659E-2</v>
       </c>
       <c r="O17" s="8">
         <f t="shared" si="5"/>
@@ -1563,15 +1566,15 @@
         <v>984</v>
       </c>
       <c r="C18" s="6">
-        <v>24500287</v>
+        <v>2450028786</v>
       </c>
       <c r="D18" s="6">
         <f t="shared" si="0"/>
-        <v>24499303</v>
+        <v>2450027802</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" si="1"/>
-        <v>0.24499303</v>
+        <v>24.50027802</v>
       </c>
       <c r="F18" s="6">
         <v>5524</v>
@@ -1583,15 +1586,15 @@
         <v>984</v>
       </c>
       <c r="I18" s="7">
-        <v>24500287</v>
+        <v>2450028786</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" si="2"/>
-        <v>24499303</v>
+        <v>2450027802</v>
       </c>
       <c r="K18" s="7">
         <f t="shared" si="3"/>
-        <v>0.24499303</v>
+        <v>24.50027802</v>
       </c>
       <c r="L18" s="7">
         <v>5524</v>
@@ -1620,15 +1623,15 @@
         <v>12950</v>
       </c>
       <c r="C19" s="6">
-        <v>40556872</v>
+        <v>4055687263</v>
       </c>
       <c r="D19" s="6">
         <f t="shared" si="0"/>
-        <v>40543922</v>
+        <v>4055674313</v>
       </c>
       <c r="E19" s="6">
         <f t="shared" si="1"/>
-        <v>0.40543921999999999</v>
+        <v>40.556743130000001</v>
       </c>
       <c r="F19" s="6">
         <v>13156</v>
@@ -1640,15 +1643,15 @@
         <v>12950</v>
       </c>
       <c r="I19" s="7">
-        <v>40556928</v>
+        <v>4056247441.8764958</v>
       </c>
       <c r="J19" s="7">
         <f t="shared" si="2"/>
-        <v>40543978</v>
+        <v>4056234491.8764958</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="3"/>
-        <v>0.40543978000000003</v>
+        <v>40.562344918764964</v>
       </c>
       <c r="L19" s="7">
         <v>13172</v>
@@ -1658,7 +1661,7 @@
       </c>
       <c r="N19" s="8">
         <f t="shared" si="4"/>
-        <v>1.3812181269656776E-4</v>
+        <v>1.3812225372760167E-2</v>
       </c>
       <c r="O19" s="8">
         <f t="shared" si="5"/>
@@ -1677,15 +1680,15 @@
         <v>2565</v>
       </c>
       <c r="C20" s="6">
-        <v>15245696</v>
+        <v>1524569632</v>
       </c>
       <c r="D20" s="6">
         <f t="shared" si="0"/>
-        <v>15243131</v>
+        <v>1524567067</v>
       </c>
       <c r="E20" s="6">
         <f t="shared" si="1"/>
-        <v>0.15243130999999999</v>
+        <v>15.245670670000001</v>
       </c>
       <c r="F20" s="6">
         <v>7948</v>
@@ -1697,15 +1700,15 @@
         <v>2565</v>
       </c>
       <c r="I20" s="7">
-        <v>15245696</v>
+        <v>1524569632</v>
       </c>
       <c r="J20" s="7">
         <f t="shared" si="2"/>
-        <v>15243131</v>
+        <v>1524567067</v>
       </c>
       <c r="K20" s="7">
         <f t="shared" si="3"/>
-        <v>0.15243130999999999</v>
+        <v>15.245670670000001</v>
       </c>
       <c r="L20" s="7">
         <v>8020</v>
@@ -1734,15 +1737,15 @@
         <v>66568</v>
       </c>
       <c r="C21" s="6">
-        <v>12975933</v>
+        <v>1297593381</v>
       </c>
       <c r="D21" s="6">
         <f t="shared" si="0"/>
-        <v>12909365</v>
+        <v>1297526813</v>
       </c>
       <c r="E21" s="6">
         <f t="shared" si="1"/>
-        <v>0.12909365</v>
+        <v>12.97526813</v>
       </c>
       <c r="F21" s="6">
         <v>23432</v>
@@ -1754,15 +1757,15 @@
         <v>66568</v>
       </c>
       <c r="I21" s="7">
-        <v>13023309</v>
+        <v>1773796385.7043729</v>
       </c>
       <c r="J21" s="7">
         <f t="shared" si="2"/>
-        <v>12956741</v>
+        <v>1773729817.7043729</v>
       </c>
       <c r="K21" s="7">
         <f t="shared" si="3"/>
-        <v>0.12956740999999999</v>
+        <v>17.737298177043726</v>
       </c>
       <c r="L21" s="7">
         <v>23592</v>
@@ -1772,7 +1775,7 @@
       </c>
       <c r="N21" s="8">
         <f t="shared" si="4"/>
-        <v>0.36698939103510497</v>
+        <v>36.700821896955489</v>
       </c>
       <c r="O21" s="8">
         <f t="shared" si="5"/>
@@ -1791,15 +1794,15 @@
         <v>13945</v>
       </c>
       <c r="C22" s="6">
-        <v>16133519</v>
+        <v>1613351913</v>
       </c>
       <c r="D22" s="6">
         <f t="shared" si="0"/>
-        <v>16119574</v>
+        <v>1613337968</v>
       </c>
       <c r="E22" s="6">
         <f t="shared" si="1"/>
-        <v>0.16119574</v>
+        <v>16.133379680000001</v>
       </c>
       <c r="F22" s="6">
         <v>3820</v>
@@ -1811,15 +1814,15 @@
         <v>13945</v>
       </c>
       <c r="I22" s="7">
-        <v>16133519</v>
+        <v>1613351913</v>
       </c>
       <c r="J22" s="7">
         <f t="shared" si="2"/>
-        <v>16119574</v>
+        <v>1613337968</v>
       </c>
       <c r="K22" s="7">
         <f t="shared" si="3"/>
-        <v>0.16119574</v>
+        <v>16.133379680000001</v>
       </c>
       <c r="L22" s="7">
         <v>3820</v>
@@ -1848,15 +1851,15 @@
         <v>25119</v>
       </c>
       <c r="C23" s="6">
-        <v>11288586</v>
+        <v>1128858651</v>
       </c>
       <c r="D23" s="6">
         <f t="shared" si="0"/>
-        <v>11263467</v>
+        <v>1128833532</v>
       </c>
       <c r="E23" s="6">
         <f t="shared" si="1"/>
-        <v>0.11263467000000001</v>
+        <v>11.28833532</v>
       </c>
       <c r="F23" s="6">
         <v>47196</v>
@@ -1868,15 +1871,15 @@
         <v>25119</v>
       </c>
       <c r="I23" s="7">
-        <v>11346186</v>
+        <v>1706143232.1826692</v>
       </c>
       <c r="J23" s="7">
         <f t="shared" si="2"/>
-        <v>11321067</v>
+        <v>1706118113.1826692</v>
       </c>
       <c r="K23" s="7">
         <f t="shared" si="3"/>
-        <v>0.11321067</v>
+        <v>17.061181131826689</v>
       </c>
       <c r="L23" s="7">
         <v>47828</v>
@@ -1886,7 +1889,7 @@
       </c>
       <c r="N23" s="8">
         <f t="shared" si="4"/>
-        <v>0.51138783466936388</v>
+        <v>51.139921416036486</v>
       </c>
       <c r="O23" s="8">
         <f t="shared" si="5"/>
@@ -1911,7 +1914,7 @@
       </c>
       <c r="N26" s="10">
         <f>GEOMEAN(N3:N4,N6,N8:N10,N12,N14,N16:N17,N19,N21,N23)</f>
-        <v>5.7900442645761312E-3</v>
+        <v>0.57901264205439873</v>
       </c>
       <c r="O26" s="10">
         <f>GEOMEAN(O3:O4,O6:O12,O14,O16:O17,O19:O21,O23)</f>
@@ -1921,6 +1924,72 @@
         <f>GEOMEAN(P2:P12,P14:P23)</f>
         <v>7.5457859483844443</v>
       </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F32" s="11"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="11"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="11"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="11"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F36" s="11"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F37" s="11"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F38" s="11"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="11"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="11"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="11"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F45" s="11"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F46" s="11"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F47" s="11"/>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F48" s="11"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F49" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>